<commit_message>
Excel File, test cases for lab.
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eadch\PycharmProjects\cs151-lab1-zain-and-ethan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0019066A-ADAB-2D40-B7F1-BC2C56C35A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF38896D-CB6C-4017-B36C-0AA976E74B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Test Description</t>
   </si>
@@ -54,9 +56,6 @@
     <t>Price is 1, we need 1 gallon</t>
   </si>
   <si>
-    <t>insert Excel formula here</t>
-  </si>
-  <si>
     <t>Zero miles, price is 1</t>
   </si>
   <si>
@@ -64,13 +63,22 @@
   </si>
   <si>
     <t>Number of miles is less than MPG</t>
+  </si>
+  <si>
+    <t>20 miles left to go, price is 2</t>
+  </si>
+  <si>
+    <t>Price is 5, we need 2 gallons</t>
+  </si>
+  <si>
+    <t>5 miles left to go, price is 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,12 +107,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,34 +133,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FFA9B7C6"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -237,6 +236,24 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color rgb="FFA9B7C6"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -251,23 +268,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E40A2E88-C760-264E-9266-04B1334E3A59}" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:E5" xr:uid="{E40A2E88-C760-264E-9266-04B1334E3A59}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E40A2E88-C760-264E-9266-04B1334E3A59}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:E8" xr:uid="{E40A2E88-C760-264E-9266-04B1334E3A59}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46024F63-9202-3A4A-A163-EF55AE6E2326}" name="Test Description" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{CB0A4D3D-327B-8948-9676-47A8A9ADBFE8}" name="in:miles" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{AC065743-B4AD-E044-B4C7-52E688AF15C6}" name="in:MPG" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{CA4C2539-BEF4-9142-9BB9-46E95ABF1149}" name="in:price" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{DA569DA6-C53A-E749-848E-C82C128C10F9}" name="out:cost"/>
+    <tableColumn id="1" xr3:uid="{46024F63-9202-3A4A-A163-EF55AE6E2326}" name="Test Description" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CB0A4D3D-327B-8948-9676-47A8A9ADBFE8}" name="in:miles" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{AC065743-B4AD-E044-B4C7-52E688AF15C6}" name="in:MPG" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{CA4C2539-BEF4-9142-9BB9-46E95ABF1149}" name="in:price" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{DA569DA6-C53A-E749-848E-C82C128C10F9}" name="out:cost">
+      <calculatedColumnFormula>(B2/C2)*D2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,22 +580,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B23E87-90D4-3B4F-8924-533CB9AAD3A2}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="26.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17">
+    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -606,35 +625,118 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="3">
+        <f>(B2/C2)*D2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E8" si="0">(B3/C3)*D3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="17">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B4" s="2">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="17">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B5" s="2">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.96666666666666667</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="17">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B6" s="2">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333326</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>